<commit_message>
update de lo que vimos ayer con el sebs
</commit_message>
<xml_diff>
--- a/data/SSC/rating_curves_SSC_Q.xlsx
+++ b/data/SSC/rating_curves_SSC_Q.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\sediment_trap_paper\data\SSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - University of Idaho\Documents\GitHub\sediment_trap_paper\data\SSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C247125C-9AF1-4F23-B0A6-EB5CD468F045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D260C226-1D0D-47F7-96C0-3622890D9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summer" sheetId="2" r:id="rId1"/>
@@ -376,11 +376,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1079,7 +1077,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2131,7 +2129,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3011,7 +3009,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4439,7 +4437,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6520,7 +6518,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7295,7 +7293,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9014,7 +9012,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9832,7 +9830,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10634,7 +10632,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11436,7 +11434,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12578,7 +12576,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13736,7 +13734,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14894,7 +14892,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15740,7 +15738,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -26843,17 +26841,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0752EAC-B958-4930-AC83-02E0D5D84BD4}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AB34" sqref="AB34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26876,904 +26874,904 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>45136.629861111112</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>110.0000003</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>2.2384712900000001</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>66.982882119999999</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <v>40.77864692</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>4.5677437518626803E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>45136.640277777777</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>53.332999999999998</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>1.261990779</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>34.389887139999999</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>17.681122080000002</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>4.5472364768501097E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>45136.650694444441</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>80.000000240000006</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>1.73032312</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>49.409612320000001</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>28.8600648</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>5.2846760713736798E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>45136.661111111112</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>43.334300550000002</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>0.6478121</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>25.369451179999999</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>17.31703727</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>4.93206577250766E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>45136.671527777777</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>92.221999819999994</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>1.9795797209999999</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>54.788411910000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>35.454008190000003</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>3.1950057445806097E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>45136.636111111111</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>99.999897899999993</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>1.7025325</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>50.927867399999997</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>47.369498</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>4.4241928267747199E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>45136.646527777775</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>105.5558544</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>2.6126065280000002</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>63.645890489999999</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>39.297357429999998</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>4.7932063047253601E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>45136.656944444447</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>50.002523099999998</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>1.7129574000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>34.066121099999997</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>14.223444600000001</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>5.7959829048480398E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>45136.667361111111</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>68.888999870000006</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>1.6975885020000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>38.772768460000002</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>28.418642909999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <v>3.6965804744147998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>45136.677777777775</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>51.112550349999999</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>1.5941184079999999</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>31.586279730000001</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>17.932152210000002</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>2.5889859461511601E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>45136.688194444447</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>45.262999909999998</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>1.0785253619999999</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>27.828759980000001</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>16.355714580000001</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>3.3731294483052898E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>45136.698611111111</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>19.999763479999999</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>0.34223409999999999</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>9.6059695600000001</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>10.05155982</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>2.0843840093555398E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>45136.719444444447</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>15.4555238</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>0.36588095999999998</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>8.3332856950000007</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>6.756357145</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>1.6196175614707702E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>45136.740277777775</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>26.000000029999999</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>0.78720007599999997</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>16.636494320000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>8.5763056340000006</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <v>1.6135680584454599E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>45136.771527777775</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>21.000042799999999</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <v>0.24858424500000001</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>8.7181228260000001</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <v>12.033335729999999</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="3">
         <v>1.45854671755473E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>45151.78125</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>76.154000150000002</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>1.535948426</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>41.556805400000002</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>33.061246330000003</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="5">
         <v>1.66432575393171E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>45151.790277777778</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>41.19999988</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>0.91580950299999997</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>23.98199936</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>16.302191019999999</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>1.6195854712328501E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>45151.793055555558</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>39.600000080000001</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>0.72662721200000002</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>21.643585559999998</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>17.229787300000002</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>1.54816878323273E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>45151.798611111109</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>27.60000003</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20">
         <v>0.53448092800000002</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>15.561848729999999</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>11.50367037</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20">
         <v>1.2900345128930501E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>45151.876388888886</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>20.833370989999999</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21">
         <v>0.47843855400000002</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>12.20871524</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>8.1462171990000005</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21">
         <v>1.48464017966453E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>45151.78125</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>43.199858990000003</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22">
         <v>0.55608318700000003</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>16.282472340000002</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>26.361303469999999</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22">
         <v>1.66432575393171E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>45151.791666666664</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>29.231349890000001</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23">
         <v>0.613805516</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>16.922344840000001</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>11.695199540000001</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23">
         <v>1.6127023508176502E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>45151.802083333336</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>25.000381399999998</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24">
         <v>0.53111522499999997</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>13.69915258</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24">
         <v>10.7701136</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24">
         <v>1.12870059393076E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>45151.8125</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>23.751649539999999</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>0.45043115</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25">
         <v>12.849270130000001</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25">
         <v>10.45194826</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25">
         <v>1.0550025930821501E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>45151.822916666664</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26">
         <v>22.22200007</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26">
         <v>0.40174336100000002</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26">
         <v>11.227002969999999</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26">
         <v>10.593253730000001</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26">
         <v>9.5114414032114996E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>45151.833333333336</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>22.222000019999999</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>0.32571578800000001</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
         <v>11.749664839999999</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27">
         <v>10.146619400000001</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27">
         <v>1.2896966402582401E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>45151.84375</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>21.904999960000001</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28">
         <v>0.26598555800000001</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28">
         <v>8.6595386179999991</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28">
         <v>12.97947578</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28">
         <v>1.1677178006885801E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>45151.854166666664</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>17.99999996</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29">
         <v>0.18115083000000001</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29">
         <v>6.5781730979999997</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29">
         <v>11.24067604</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29">
         <v>1.28897170412782E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>45151.864583333336</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30">
         <v>20.498955209999998</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30">
         <v>0.41792718899999998</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30">
         <v>11.0970862</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30">
         <v>8.9839418159999997</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30">
         <v>1.5147430220548E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>45151.875</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31">
         <v>12.5580333</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31">
         <v>0.22869155199999999</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>7.1097737370000003</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31">
         <v>5.2195680150000001</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31">
         <v>1.5147430220548E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>45151.885416666664</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>18.000547560000001</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32">
         <v>0.38789038799999997</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>10.00057462</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32">
         <v>7.6120825500000002</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32">
         <v>1.28897170412782E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>45151.895833333336</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="3">
         <v>20.000629279999998</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="3">
         <v>0.40784703999999999</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="3">
         <v>10.445131399999999</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="3">
         <v>9.1476508400000007</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="3">
         <v>1.1670477158377801E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
         <v>45166.513888888891</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="5">
         <v>77.894999929999997</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="5">
         <v>1.1431815679999999</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <v>37.685186520000002</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="5">
         <v>39.066631839999999</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="5">
         <v>1.3918048948303501E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>45166.524305555555</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35">
         <v>43.00000009</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35">
         <v>0.58630581699999995</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
         <v>20.068511470000001</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <v>22.3451828</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35">
         <v>1.29054690999993E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>45166.534722222219</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36">
         <v>36</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36">
         <v>0.63156193199999999</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
         <v>19.97190904</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36">
         <v>15.39652903</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36">
         <v>1.2070389853395799E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>45166.545138888891</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>28.8362148</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37">
         <v>0.50938818900000005</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37">
         <v>14.830492660000001</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37">
         <v>13.49633395</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37">
         <v>1.1684788928497499E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>45166.555555555555</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38">
         <v>29.545192100000001</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38">
         <v>0.48133913299999997</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
         <v>15.63631633</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38">
         <v>13.42753665</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38">
         <v>1.24889235123712E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>45166.586805555555</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39">
         <v>26.841154079999999</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39">
         <v>0.50269211800000002</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39">
         <v>14.121905659999999</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39">
         <v>12.216556300000001</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39">
         <v>1.28897170412782E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>45166.607638888891</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="3">
         <v>24.00051874</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="3">
         <v>0.435763128</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="3">
         <v>13.756626860000001</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="3">
         <v>9.8081287439999993</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="3">
         <v>1.3063574865192801E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45183.744444444441</v>
       </c>
@@ -27796,7 +27794,7 @@
         <v>2.4210236431668801E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45183.754861111112</v>
       </c>
@@ -27819,7 +27817,7 @@
         <v>2.26863815215868E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45183.765277777777</v>
       </c>
@@ -27842,7 +27840,7 @@
         <v>1.52396285400846E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45183.786111111112</v>
       </c>
@@ -27865,7 +27863,7 @@
         <v>1.44609417106578E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45183.79791666667</v>
       </c>
@@ -27888,7 +27886,7 @@
         <v>1.42155690608048E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45183.739583333336</v>
       </c>
@@ -27911,7 +27909,7 @@
         <v>2.0528229072998699E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45183.75</v>
       </c>
@@ -27934,7 +27932,7 @@
         <v>2.8418244841577602E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45183.760416666664</v>
       </c>
@@ -27957,7 +27955,7 @@
         <v>1.6135680584454599E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45183.78125</v>
       </c>
@@ -27980,7 +27978,7 @@
         <v>1.4675642779279199E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45183.802083333336</v>
       </c>
@@ -28013,16 +28011,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -28048,501 +28046,501 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>45033.6875</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>23.16</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2">
         <v>205</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>0.16876276700000001</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <v>9.6563256909999993</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>13.333347699999999</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
         <v>0.171886328011326</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>45033.854166666664</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>15</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>206</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>0.18973258500000001</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>9.3864923250000007</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>5.4255319049999997</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3">
         <v>0.17858253626276399</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>45034.020833333336</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>8.9499999999999993</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4">
         <v>222</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>5.6863955000000001E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>4.070310299</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>4.821338066</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
         <v>0.17366943358482301</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>45034.1875</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>9.5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>207</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>7.6635030000000007E-2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>4.4512997969999999</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>4.9726531850000004</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>0.16965170896000101</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>45034.6875</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>23</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>225</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>0.31997206700000003</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>14.03493842</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>8.647427231</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <v>0.184383366461084</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>45034.895833333336</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>226</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>0.12516511499999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>5.7027741150000004</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>9.1720607699999999</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <v>0.18482722940617299</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>45035.104166666664</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>227</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>6.8218310000000004E-2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>4.4745853200000001</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>5.4571963700000001</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <v>0.17679177852632699</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>45035.520833333336</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>3.5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>229</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>2.8156476999999999E-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>1.8744080279999999</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>1.597280875</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <v>0.17366943358482301</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>45037.395833333336</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>6.25</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>234</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>5.7663182E-2</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>2.9218879169999998</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <v>3.269588277</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <v>0.176808528840387</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>45046.75</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>42</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>323</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>0.53259914399999997</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>17.814978010000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>23.653744549999999</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <v>0.18666898145639299</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>45046.958333333336</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>17.420000000000002</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>324</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>0.152104448</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>6.5842968209999997</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>10.682395939999999</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <v>0.186683051720204</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>45047.583333333336</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>327</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>7.5044879999999994E-2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>3.1020945539999998</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>2.8228605720000002</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13">
         <v>0.18257120581726999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>45047.833333333336</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>22.14</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>343</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>0.20720609000000001</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>7.1975824179999996</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14">
         <v>14.736734999999999</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
         <v>0.198135555256964</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>45048.125</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>344</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>0.15141339000000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>4.4648754400000001</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15">
         <v>5.3823117800000002</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15">
         <v>0.202196770380911</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>45048.416666666664</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>6.43</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>345</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>0.109183207</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>2.6773267500000002</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16">
         <v>3.6426933610000001</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16">
         <v>0.19323818890813499</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>45048.708333333336</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>18</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>346</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>0.21313927799999999</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>7.1794649880000003</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17">
         <v>10.603855210000001</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17">
         <v>0.228024805885122</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>45049.833333333336</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>20.67</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>350</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>0.25397928400000003</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>7.6876070329999999</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18">
         <v>12.72601482</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18">
         <v>0.277136428383431</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>45050.083333333336</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>11.88</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19">
         <v>351</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>0.117770526</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>5.1492537199999999</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>6.60844217</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <v>0.26457163552462398</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>45050.958333333336</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>7.14</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="3">
         <v>356</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>0</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="3">
         <v>4.2890389799999999</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="3">
         <v>2.8530971690000002</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="3">
         <v>0.24797493203292101</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45034.6875</v>
       </c>
@@ -28568,7 +28566,7 @@
         <v>0.184383366461084</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45034.895833333336</v>
       </c>
@@ -28594,7 +28592,7 @@
         <v>0.18482722940617299</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45035.104166666664</v>
       </c>
@@ -28620,7 +28618,7 @@
         <v>0.17679177852632699</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45035.3125</v>
       </c>
@@ -28646,7 +28644,7 @@
         <v>0.17278170769464399</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45035.9375</v>
       </c>
@@ -28672,7 +28670,7 @@
         <v>0.19405093533895701</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45036.145833333336</v>
       </c>
@@ -28698,7 +28696,7 @@
         <v>0.19159893063024599</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45036.979166666664</v>
       </c>
@@ -28724,7 +28722,7 @@
         <v>0.181738892085264</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45037.8125</v>
       </c>
@@ -28750,7 +28748,7 @@
         <v>0.16521002777305599</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45038.229166666664</v>
       </c>
@@ -28776,7 +28774,7 @@
         <v>0.16105877013360401</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45038.645833333336</v>
       </c>
@@ -28802,7 +28800,7 @@
         <v>0.15938753872582101</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45038.854166666664</v>
       </c>
@@ -28828,7 +28826,7 @@
         <v>0.16105877013360401</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45040.083333333336</v>
       </c>
@@ -28854,7 +28852,7 @@
         <v>0.17433150869914599</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45040.708333333336</v>
       </c>
@@ -28880,7 +28878,7 @@
         <v>0.18995671353775601</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45040.916666666664</v>
       </c>
@@ -28906,7 +28904,7 @@
         <v>0.18995671353775601</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45044.666666666664</v>
       </c>
@@ -28932,7 +28930,7 @@
         <v>0.15354232467829301</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45046.541666666664</v>
       </c>
@@ -28958,7 +28956,7 @@
         <v>0.169350687476575</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45046.75</v>
       </c>
@@ -28984,7 +28982,7 @@
         <v>0.18666898145639299</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45047.833333333336</v>
       </c>
@@ -29010,7 +29008,7 @@
         <v>0.198135555256964</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45049.583333333336</v>
       </c>
@@ -29036,7 +29034,7 @@
         <v>0.21435307565376299</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45049.833333333336</v>
       </c>
@@ -29062,7 +29060,7 @@
         <v>0.277136428383431</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45050.833333333336</v>
       </c>
@@ -29088,7 +29086,7 @@
         <v>0.25114191513496997</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45050.958333333336</v>
       </c>
@@ -29114,7 +29112,7 @@
         <v>0.24797493203292101</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45051.458333333336</v>
       </c>

</xml_diff>